<commit_message>
Ready for test again
</commit_message>
<xml_diff>
--- a/Driving_Notes.xlsx
+++ b/Driving_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashraf/Documents/Github/behavioral_profiling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A1BC85-8804-4A4A-9D0A-62631238848D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6B771B-5459-CE4F-B635-FAC2B98D41B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" activeTab="2" xr2:uid="{CE62AA09-BCB8-FF42-8315-43245B711082}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" activeTab="3" xr2:uid="{CE62AA09-BCB8-FF42-8315-43245B711082}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Sheet 4" sheetId="7" r:id="rId4"/>
     <sheet name="Sheet 5" sheetId="9" r:id="rId5"/>
     <sheet name="Sheet 6" sheetId="10" r:id="rId6"/>
+    <sheet name="Sheet 7" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet 8" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="75">
   <si>
     <t>Interest Points</t>
   </si>
@@ -1430,7 +1432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEED39CA-117A-8847-BB2E-82C9A3B198C5}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1842,8 +1844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA2BA50-2B95-FF43-9FC6-142C482326A9}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2631,4 +2633,534 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC8841-5808-9244-A5AE-9A821460627E}">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" style="5" customWidth="1"/>
+    <col min="4" max="12" width="50.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C23065-D40B-374D-B96F-802F16110DDE}">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" style="5" customWidth="1"/>
+    <col min="4" max="12" width="50.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>